<commit_message>
Updated doc to be aligned with HW
</commit_message>
<xml_diff>
--- a/doc/CL_DMA_reference.xlsx
+++ b/doc/CL_DMA_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -44,67 +44,67 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="217">
   <si>
-    <t>Document Information</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>CL_DMA reference</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>IP reference</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>Florent Rotenberg</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Fisrt Release</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>CL_DMA interface definition</t>
-  </si>
-  <si>
-    <t>IP Information</t>
-  </si>
-  <si>
-    <t>IP type</t>
-  </si>
-  <si>
-    <t>CL_DMA</t>
-  </si>
-  <si>
-    <t>Delivery Type</t>
-  </si>
-  <si>
-    <t>History</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Modification</t>
-  </si>
-  <si>
-    <t>26/10/2016</t>
+    <t xml:space="preserve">Document Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL_DMA reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florent Rotenberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fisrt Release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL_DMA interface definition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL_DMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">History</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/10/2016</t>
   </si>
   <si>
     <r>
@@ -115,7 +115,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>1</t>
+      <t xml:space="preserve">1</t>
     </r>
     <r>
       <rPr>
@@ -126,7 +126,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>st</t>
+      <t xml:space="preserve">st</t>
     </r>
     <r>
       <rPr>
@@ -136,613 +136,613 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>release</t>
+      <t xml:space="preserve">release</t>
     </r>
   </si>
   <si>
-    <t>F.Rotenberg</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
-    <t>Info</t>
-  </si>
-  <si>
-    <t>This sheet. General information about document usage</t>
-  </si>
-  <si>
-    <t>Usage</t>
-  </si>
-  <si>
-    <t>Guidelines on how to used the various sheet</t>
-  </si>
-  <si>
-    <t>IP Release</t>
-  </si>
-  <si>
-    <t>Release information sheet describing</t>
-  </si>
-  <si>
-    <t>IPIF_relx.x</t>
-  </si>
-  <si>
-    <t>IP interface description reference, describing IP symbol/entity and integration and test information relative to IP interface.</t>
-  </si>
-  <si>
-    <t>IPDESCR_Relx.x</t>
-  </si>
-  <si>
-    <t>Description of the main features of the IP</t>
-  </si>
-  <si>
-    <t>IPREGLIST_rely.y</t>
-  </si>
-  <si>
-    <t>Description of the list of registers used by IP. Registers can be physically instanciated inside IP or outside IP.</t>
-  </si>
-  <si>
-    <t>IPREGMAP_relz.z</t>
-  </si>
-  <si>
-    <t>Description of mapping of bit fields when registers are internal to IP. This sheet is optional for IP which are not instanciating registers as information can be build from IPIF and IPRELIST sheet.</t>
-  </si>
-  <si>
-    <t>IPTREGMAP_relz.z</t>
-  </si>
-  <si>
-    <t>Description of mapping of test bit field when registers are internal to IP. This sheet is optional for IP which are not instanciating registers as information can be build from IPIF and IPRELIST sheet.</t>
-  </si>
-  <si>
-    <t>IPUDMACMDLIST_relz.z</t>
-  </si>
-  <si>
-    <t>Description of IP UDMA commands list used by IP.</t>
-  </si>
-  <si>
-    <t>IPUDMACMDMAP_relz.z</t>
-  </si>
-  <si>
-    <t>Description of mapping of bit fields in IP UDMA commands used by IP.</t>
-  </si>
-  <si>
-    <t>IP Release Sheet</t>
-  </si>
-  <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>Possible Value</t>
-  </si>
-  <si>
-    <t>IP release version numeroted as [major release].[minor release]. A release is major whenever IP interface is modified.</t>
-  </si>
-  <si>
-    <t>X.Y. Z</t>
-  </si>
-  <si>
-    <t>Release description</t>
-  </si>
-  <si>
-    <t>This is a free text entry expliciting the release main modifications and purpose.</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>IPIF</t>
-  </si>
-  <si>
-    <t>IPIF sheet version to be used for this release.</t>
-  </si>
-  <si>
-    <t>IPDESCR</t>
-  </si>
-  <si>
-    <t>IPDESCR sheet version to nbe used for this release</t>
-  </si>
-  <si>
-    <t>X.Y.Z</t>
-  </si>
-  <si>
-    <t>IPREGLIST</t>
-  </si>
-  <si>
-    <t>IPREGLIST sheet version to be used for this release.</t>
-  </si>
-  <si>
-    <t>IPREGMAP</t>
-  </si>
-  <si>
-    <t>IPREGMAP sheet version to be used for this release.</t>
-  </si>
-  <si>
-    <t>IPUDMACMDLIST</t>
-  </si>
-  <si>
-    <t>IPUDMACMDLIST sheet version to be used for this release.</t>
-  </si>
-  <si>
-    <t>IPUDMACMDMAP</t>
-  </si>
-  <si>
-    <t>IPUDMACMDMAP sheet version to be used for this release.</t>
-  </si>
-  <si>
-    <t>IPDOC</t>
-  </si>
-  <si>
-    <t>IPDOC version to be used for this release.</t>
-  </si>
-  <si>
-    <t>GIT version</t>
-  </si>
-  <si>
-    <t>GIT database number corresponding to IP design code and IP reference XLS.</t>
-  </si>
-  <si>
-    <t>Integer</t>
-  </si>
-  <si>
-    <t>IPIF sheet</t>
-  </si>
-  <si>
-    <t>IP Interface description</t>
-  </si>
-  <si>
-    <t>IP Pin Name</t>
-  </si>
-  <si>
-    <t>Name of IP Pin. This must must exactly name find in code or schematic (including case).</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>Direction or type of signal</t>
-  </si>
-  <si>
-    <t>In,Out,IO</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Analog, Digital, supply, DR (Dual Rail), SR (SingleRail)</t>
-  </si>
-  <si>
-    <t>Analog,Digital, VDD, GND, DR, SR</t>
-  </si>
-  <si>
-    <t>Voltage Domain</t>
-  </si>
-  <si>
-    <t>Clock domain</t>
-  </si>
-  <si>
-    <t>IO</t>
-  </si>
-  <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>Reset Value</t>
-  </si>
-  <si>
-    <t>Integration information</t>
-  </si>
-  <si>
-    <t>Integration comment</t>
-  </si>
-  <si>
-    <t>Core Interface</t>
-  </si>
-  <si>
-    <t>Register  Interface</t>
-  </si>
-  <si>
-    <t>Register name</t>
-  </si>
-  <si>
-    <t>DFT value</t>
-  </si>
-  <si>
-    <t>Level Shifter</t>
-  </si>
-  <si>
-    <t>Isolation cell</t>
-  </si>
-  <si>
-    <t>Connected to</t>
-  </si>
-  <si>
-    <t>Load</t>
-  </si>
-  <si>
-    <t>Drive</t>
-  </si>
-  <si>
-    <t>Destination supply</t>
-  </si>
-  <si>
-    <t>Hard Macro information</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>layer</t>
-  </si>
-  <si>
-    <t>Antenna</t>
-  </si>
-  <si>
-    <t>Additonal Information</t>
-  </si>
-  <si>
-    <t>FreeText 1</t>
-  </si>
-  <si>
-    <t>FreeText 2</t>
-  </si>
-  <si>
-    <t>Driver information</t>
-  </si>
-  <si>
-    <t>Function1</t>
-  </si>
-  <si>
-    <t>Function2</t>
-  </si>
-  <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
-    <t>Rel1.0.0</t>
-  </si>
-  <si>
-    <t>1.1.0</t>
-  </si>
-  <si>
-    <t>Extended 2D COUNT and STRIDE to 32-bit, updated configuration FSM</t>
-  </si>
-  <si>
-    <t>Bit position</t>
-  </si>
-  <si>
-    <t>Trim during production</t>
-  </si>
-  <si>
-    <t>Cluster DMA component manages the following features:
+    <t xml:space="preserve">F.Rotenberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This sheet. General information about document usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guidelines on how to used the various sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Release information sheet describing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPIF_relx.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP interface description reference, describing IP symbol/entity and integration and test information relative to IP interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDESCR_Relx.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of the main features of the IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGLIST_rely.y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of the list of registers used by IP. Registers can be physically instanciated inside IP or outside IP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGMAP_relz.z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of mapping of bit fields when registers are internal to IP. This sheet is optional for IP which are not instanciating registers as information can be build from IPIF and IPRELIST sheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPTREGMAP_relz.z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of mapping of test bit field when registers are internal to IP. This sheet is optional for IP which are not instanciating registers as information can be build from IPIF and IPRELIST sheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPUDMACMDLIST_relz.z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of IP UDMA commands list used by IP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPUDMACMDMAP_relz.z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of mapping of bit fields in IP UDMA commands used by IP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Release Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possible Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP release version numeroted as [major release].[minor release]. A release is major whenever IP interface is modified.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X.Y. Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Release description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a free text entry expliciting the release main modifications and purpose.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPIF sheet version to be used for this release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDESCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDESCR sheet version to nbe used for this release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X.Y.Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGLIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGLIST sheet version to be used for this release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGMAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGMAP sheet version to be used for this release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPUDMACMDLIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPUDMACMDLIST sheet version to be used for this release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPUDMACMDMAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPUDMACMDMAP sheet version to be used for this release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDOC version to be used for this release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIT version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIT database number corresponding to IP design code and IP reference XLS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPIF sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Interface description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Pin Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of IP Pin. This must must exactly name find in code or schematic (including case).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction or type of signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In,Out,IO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog, Digital, supply, DR (Dual Rail), SR (SingleRail)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog,Digital, VDD, GND, DR, SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage Domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clock domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integration information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integration comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register  Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFT value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level Shifter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isolation cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connected to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hard Macro information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antenna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additonal Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FreeText 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FreeText 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driver information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rel1.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extended 2D COUNT and STRIDE to 32-bit, updated configuration FSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trim during production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster DMA component manages the following features:
 - parametric number of RX/TX full-duplex channels
 - Up to 16 outstanding transfers between L1 and L2 memories
 - Linear or 2D transfers modes on both TCDM or EXT (L2) sides</t>
   </si>
   <si>
-    <t>Register Name</t>
-  </si>
-  <si>
-    <t>Header</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Register Type</t>
-  </si>
-  <si>
-    <t>Host Access Type</t>
-  </si>
-  <si>
-    <t>Host access bus</t>
-  </si>
-  <si>
-    <t>IP access Type</t>
-  </si>
-  <si>
-    <t>Default Value</t>
-  </si>
-  <si>
-    <t>FootNote</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>CMD</t>
-  </si>
-  <si>
-    <t>0x0</t>
-  </si>
-  <si>
-    <t>Config</t>
-  </si>
-  <si>
-    <t>R/W</t>
-  </si>
-  <si>
-    <t>DEMUX</t>
-  </si>
-  <si>
-    <t>Cluster DMA configuration register.</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>0x4</t>
-  </si>
-  <si>
-    <t>Cluster DMA status register.</t>
-  </si>
-  <si>
-    <t>Bit field</t>
-  </si>
-  <si>
-    <t>Register</t>
-  </si>
-  <si>
-    <t>Bit Position</t>
-  </si>
-  <si>
-    <t>Format is operation dependent. See below.</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Format Name</t>
-  </si>
-  <si>
-    <t>Next State</t>
-  </si>
-  <si>
-    <t>Start graph</t>
-  </si>
-  <si>
-    <t>Graph title</t>
-  </si>
-  <si>
-    <t>IDLE</t>
-  </si>
-  <si>
-    <t>GET_TID</t>
-  </si>
-  <si>
-    <t>ID_ACK</t>
-  </si>
-  <si>
-    <t>Queue transaction with ID</t>
-  </si>
-  <si>
-    <t>CMD_ACK</t>
-  </si>
-  <si>
-    <t>Queue transaction without ID</t>
-  </si>
-  <si>
-    <t>Get DMA status</t>
-  </si>
-  <si>
-    <t>FREE_TID</t>
-  </si>
-  <si>
-    <t>Free DMA transfer</t>
-  </si>
-  <si>
-    <t>TCDM_ADDR</t>
-  </si>
-  <si>
-    <t>TCDM_ACK</t>
-  </si>
-  <si>
-    <t>TCDM_ADDR_ACK</t>
-  </si>
-  <si>
-    <t>EXT_ADDR</t>
-  </si>
-  <si>
-    <t>EXT_ADDR_ACK</t>
-  </si>
-  <si>
-    <t>- </t>
-  </si>
-  <si>
-    <t>TRANSFER NOT 2D</t>
-  </si>
-  <si>
-    <t>2D_EXT_COUNT</t>
-  </si>
-  <si>
-    <t>EXT_COUNT_ACK</t>
-  </si>
-  <si>
-    <t>TRANSFER 2D ON EXT INTERFACE</t>
-  </si>
-  <si>
-    <t>2D_TCDM_COUNT</t>
-  </si>
-  <si>
-    <t>TCDM_COUNT_ACK</t>
-  </si>
-  <si>
-    <t>TRANSFER 2D ON TCDM INTERFACE</t>
-  </si>
-  <si>
-    <t>2D_EXT_STRIDE</t>
-  </si>
-  <si>
-    <t>EXT_STRIDE_ACK</t>
-  </si>
-  <si>
-    <t>TRANSFER NOT 2D ON TCDM INTERFACE</t>
-  </si>
-  <si>
-    <t>2D_TCDM_STRIDE</t>
-  </si>
-  <si>
-    <t>TCDM_STRIDE_ACK</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>Cluster DMA transfer identifier format.</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>Cluster DMA transfer configuration format.</t>
-  </si>
-  <si>
-    <t>Cluster DMA L1 base address configuration format.</t>
-  </si>
-  <si>
-    <t>Cluster DMA L2  base address configuration format.</t>
-  </si>
-  <si>
-    <t>Cluster DMA 2D transfer external count.</t>
-  </si>
-  <si>
-    <t>Cluster DMA 2D transfer external stride.</t>
-  </si>
-  <si>
-    <t>Cluster DMA 2D transfer tcdm count.</t>
-  </si>
-  <si>
-    <t>Cluster DMA 2D transfer tcdm stride.</t>
-  </si>
-  <si>
-    <t>Cluster DMA transfer free command format.</t>
-  </si>
-  <si>
-    <t>Cluster DMA transfer status format.</t>
-  </si>
-  <si>
-    <t>LEN</t>
-  </si>
-  <si>
-    <t>Transfer length in bytes configuration bitfield.</t>
-  </si>
-  <si>
-    <t>TYPE</t>
-  </si>
-  <si>
-    <t>Transfer direction configuration bitfield:
+    <t xml:space="preserve">Register Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Host Access Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Host access bus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP access Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FootNote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R/W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEMUX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster DMA configuration register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster DMA status register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Format is operation dependent. See below.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Format Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graph title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GET_TID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID_ACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queue transaction with ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_ACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queue transaction without ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get DMA status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FREE_TID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free DMA transfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCDM_ADDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCDM_ACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCDM_ADDR_ACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXT_ADDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXT_ADDR_ACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSFER NOT 2D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D_EXT_COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXT_COUNT_ACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSFER 2D ON EXT INTERFACE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D_TCDM_COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCDM_COUNT_ACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSFER 2D ON TCDM INTERFACE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D_EXT_STRIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXT_STRIDE_ACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSFER NOT 2D ON TCDM INTERFACE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D_TCDM_STRIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCDM_STRIDE_ACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster DMA transfer identifier format.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster DMA transfer configuration format.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster DMA L1 base address configuration format.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster DMA L2  base address configuration format.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster DMA 2D transfer external count.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster DMA 2D transfer external stride.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster DMA 2D transfer tcdm count.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster DMA 2D transfer tcdm stride.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster DMA transfer free command format.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster DMA transfer status format.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer length in bytes configuration bitfield.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer direction configuration bitfield:
 - 1'b0: L1 to L2
 - 1'b1: L2 to L2</t>
   </si>
   <si>
-    <t>INC</t>
-  </si>
-  <si>
-    <t>Transfer incremental configuration bitfield:
+    <t xml:space="preserve">INC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer incremental configuration bitfield:
 - 1'b0: non incremental
 - 1'b1: incremental</t>
   </si>
   <si>
-    <t>2D EXT</t>
-  </si>
-  <si>
-    <t>Transfer type configuration bitfield:
+    <t xml:space="preserve">2D EXT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer type configuration bitfield:
 - 1'b0: linear transfer in EXT interface
 - 1'b1: 2D transfer in EXT interface</t>
   </si>
   <si>
-    <t>ELE</t>
-  </si>
-  <si>
-    <t>Transfer event generation configuration bitfield:
+    <t xml:space="preserve">ELE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer event generation configuration bitfield:
 - 1'b0: disabled
 - 1'b1: enabled</t>
   </si>
   <si>
-    <t>ILE</t>
-  </si>
-  <si>
-    <t>Transfer interrupt generation configuration bitfield:
+    <t xml:space="preserve">ILE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer interrupt generation configuration bitfield:
 - 1'b0: disabled
 - 1'b1: enabled</t>
   </si>
   <si>
-    <t>BLE</t>
-  </si>
-  <si>
-    <t>Transfer event or interrupt broadcast configuration bitfield:
+    <t xml:space="preserve">BLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer event or interrupt broadcast configuration bitfield:
 - 1'b0: event or interrupt is routed to the cluster core who initiated the transfer
 - 1'b1: event or interrupt are broadcasted to all cluster cores</t>
   </si>
   <si>
-    <t>2D TCDM</t>
-  </si>
-  <si>
-    <t>Transfer type configuration bitfield:
+    <t xml:space="preserve">2D TCDM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer type configuration bitfield:
 - 1'b0: linear transfer in TCDM interface
 - 1'b1: 2D transfer in TCDM interface</t>
   </si>
   <si>
-    <t>TID</t>
-  </si>
-  <si>
-    <t>Transfer identifier value bitfield.</t>
-  </si>
-  <si>
-    <t>ADDR</t>
-  </si>
-  <si>
-    <t>Transfer L1 base address configuration bitfield.</t>
-  </si>
-  <si>
-    <t>Transfer L2 base address configuration bitfield.</t>
-  </si>
-  <si>
-    <t>2D EXT COUNT</t>
-  </si>
-  <si>
-    <t>EXT 2D transfer conut value configuration bitfield.</t>
-  </si>
-  <si>
-    <t>2D EXT STRIDE</t>
-  </si>
-  <si>
-    <t>EXT 2D transfer stride value configuration bitfield.</t>
-  </si>
-  <si>
-    <t>2D TCDM COUNT</t>
-  </si>
-  <si>
-    <t>TCDM 2D transfer conut value configuration bitfield.</t>
-  </si>
-  <si>
-    <t>2D TCDM STRIDE</t>
-  </si>
-  <si>
-    <t>TCDM 2D transfer stride value configuration bitfield.</t>
-  </si>
-  <si>
-    <t>TID_TR</t>
-  </si>
-  <si>
-    <t>Transfer status bitfield:
+    <t xml:space="preserve">TID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer identifier value bitfield.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer L1 base address configuration bitfield.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer L2 base address configuration bitfield.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D EXT COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXT 2D transfer conut value configuration bitfield.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D EXT STRIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXT 2D transfer stride value configuration bitfield.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D TCDM COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCDM 2D transfer conut value configuration bitfield.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D TCDM STRIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCDM 2D transfer stride value configuration bitfield.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TID_TR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer status bitfield:
 TID_TR[i]=1'b1 means that transfer with TID i is active.</t>
   </si>
   <si>
-    <t>TID_ALLOC</t>
-  </si>
-  <si>
-    <t>Transfer status bitfield:
+    <t xml:space="preserve">TID_ALLOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer status bitfield:
 - TID_TR[i]=1'b0 means that transfer allocator with TID i-16 is free.
 - TID_TR[i]=1'b1 means that transfer allocator with TID i-16 is reserved.</t>
   </si>
   <si>
-    <t>TID_FREE</t>
-  </si>
-  <si>
-    <t>Transfer canceller configuration bitfield. Writing a 1'b1 in TID_FREE[i] will free transfer with TID i.</t>
-  </si>
-  <si>
-    <t>testcase location&amp;name</t>
+    <t xml:space="preserve">TID_FREE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer canceller configuration bitfield. Writing a 1'b1 in TID_FREE[i] will free transfer with TID i.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testcase location&amp;name</t>
   </si>
 </sst>
 </file>
@@ -750,7 +750,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -1316,10 +1316,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.0890688259109"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="38.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,22 +1625,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="68.9795918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.6275303643725"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="73.4817813765182"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="8.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,7 +1686,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="58" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="61" t="s">
         <v>171</v>
@@ -1712,7 +1712,7 @@
         <v>124</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="58" t="n">
         <v>1</v>
@@ -1741,7 +1741,7 @@
         <v>124</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="58" t="n">
         <v>1</v>
@@ -1770,7 +1770,7 @@
         <v>124</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" s="58" t="n">
         <v>1</v>
@@ -1799,7 +1799,7 @@
         <v>124</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="58" t="n">
         <v>1</v>
@@ -1828,7 +1828,7 @@
         <v>124</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" s="58" t="n">
         <v>1</v>
@@ -1857,7 +1857,7 @@
         <v>124</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E8" s="58" t="n">
         <v>1</v>
@@ -1886,7 +1886,7 @@
         <v>124</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E9" s="58" t="n">
         <v>1</v>
@@ -2219,11 +2219,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.42914979757085"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.03238866396761"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2672064777328"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.42914979757085"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.62753036437247"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2264,11 +2264,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="38.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.2672064777328"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="41.3967611336032"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="28.5425101214575"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.90688259109312"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2644,12 +2644,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="58.3163265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.90688259109312"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="62.1295546558704"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="1" width="9.90688259109312"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="1" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="9.90688259109312"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2740,16 +2740,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="2" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="21" min="16" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1017" min="23" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="8" min="2" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.3724696356275"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.0202429149798"/>
+    <col collapsed="false" hidden="false" max="21" min="16" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1017" min="23" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3927,8 +3927,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="58" width="189.663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="58" width="202.085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3967,18 +3966,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.3157894736842"/>
     <col collapsed="false" hidden="true" max="2" min="2" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="3.64285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="43.1989795918367"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="39.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="3.8582995951417"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.0323886639676"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.1255060728745"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="46.0121457489879"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="42.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="8.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4128,16 +4127,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="68.9795918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.6275303643725"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="73.4817813765182"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4243,13 +4242,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="58" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="58" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="58" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="58" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="58" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="58" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="58" width="24.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="58" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.0971659919028"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4498,16 +4497,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.3724696356275"/>
     <col collapsed="false" hidden="true" max="2" min="2" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="3.64285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="57.9132653061224"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="39.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1017" min="9" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="3.8582995951417"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="61.6518218623482"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="42.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1017" min="9" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>